<commit_message>
[master] Removed all hard coded web domains in asset paths
</commit_message>
<xml_diff>
--- a/src/Components/data/wx-images.xlsx
+++ b/src/Components/data/wx-images.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maysamheydari/amagi-poc/src/Components/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C2090BC-3078-FD49-8472-5965653D9615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D104D138-B40B-2848-96EF-CC971166BA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="11840" windowWidth="38400" windowHeight="21600" xr2:uid="{27725300-7AC2-F649-856A-4042AE1EE323}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="204">
   <si>
     <t>site</t>
   </si>
@@ -332,6 +332,321 @@
   </si>
   <si>
     <t>WJAX</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/5day.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Auglaize%20Co%20Temps.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Auglaize%20Co%20Today.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Auglaize%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Butler%20Co%20Temps%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Butler%20Co%20Today.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Butler%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Champaign%20Co%20Temperatures.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Champaign%20Co%20Today.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Champain%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Clark%20Co%20Temps.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Clark%20Co%20Today%20.png</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Clark%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Darke%20Co%20Temps.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Darke%20Co%20Today%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Darke%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/DMA%20Visibility.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/DMA%20Watches%20Warnings.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Greene%20Co%20Temps%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Greene%20Co%20Today.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Greene%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Live%20Doppler%207.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Logan%20Co%20Temps%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Logan%20Co%20Today.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Logan%20County%20Radar.png</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Mercer%20Co%20Temps%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Mercer%20Co%20Today%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Mercer%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Miami%20Co%20Temps.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Miami%20Co%20Today.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Miami%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Miami%20Valley%20Temps.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Miami%20Valley%20Wind%20Speed.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Montgomery%20Co%20Temps%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Montgomery%20Co%20Today.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Montgomery%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/National%20Airport%20Delays.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/National%20SatRad.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Preble%20Co%20Temps.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Preble%20Co%20Today.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Preble%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Redional%20SatRad%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Regional%20Airport%20Delays.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Shelby%20Co%20Temps%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Shelby%20Co%20Today%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Shelby%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Warren%20Co%20Temps%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Warren%20Co%20Today.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Warren%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Wayne%20Co%20Temps.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Wayne%20Co%20Today%20.jpg</t>
+  </si>
+  <si>
+    <t>https://mediaweb.whio.com/weather/Wayne%20County%20Radar.jpg</t>
+  </si>
+  <si>
+    <t>5-day forecast</t>
+  </si>
+  <si>
+    <t>Auglaize County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Auglaize County: County Forecast</t>
+  </si>
+  <si>
+    <t>Auglaize County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Butler County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Butler County: County Forecast</t>
+  </si>
+  <si>
+    <t>Butler County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Champaign County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Champaign County: County Forecast</t>
+  </si>
+  <si>
+    <t>Champaign County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Clark County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Clark County: County Forecast</t>
+  </si>
+  <si>
+    <t>Clark County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Darke County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Darke County: County Forecast</t>
+  </si>
+  <si>
+    <t>Darke County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Miami Valley Visbility</t>
+  </si>
+  <si>
+    <t>Current Alerts</t>
+  </si>
+  <si>
+    <t>Greene County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Greene County: County Forecast</t>
+  </si>
+  <si>
+    <t>Greene County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Live Doppler 7</t>
+  </si>
+  <si>
+    <t>Logan County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Logan County: County Forecast</t>
+  </si>
+  <si>
+    <t>Logan County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Mercer County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Mercer County: County Forecast</t>
+  </si>
+  <si>
+    <t>Mercer County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Miami County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Miami County: County Forecast</t>
+  </si>
+  <si>
+    <t>Miami County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Miami Valley Temperatures</t>
+  </si>
+  <si>
+    <t>Miami Vallery Wind Speed &amp; Direction</t>
+  </si>
+  <si>
+    <t>Montgomery County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Montgomery County: County Forecast</t>
+  </si>
+  <si>
+    <t>Montgomery County: Live Doppler</t>
+  </si>
+  <si>
+    <t>National Airport Delays</t>
+  </si>
+  <si>
+    <t>National Satellite &amp; Radar</t>
+  </si>
+  <si>
+    <t>Preble County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Preble County: County Forecast</t>
+  </si>
+  <si>
+    <t>Preble County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Regional Satellite &amp; Radar</t>
+  </si>
+  <si>
+    <t>Regional Airport Delays</t>
+  </si>
+  <si>
+    <t>Shelby County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Shelby County: County Forecast</t>
+  </si>
+  <si>
+    <t>Shelby County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Warren County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Warren County: County Forecast</t>
+  </si>
+  <si>
+    <t>Warren County: Live Doppler</t>
+  </si>
+  <si>
+    <t>Wayne County: Current Temperatures</t>
+  </si>
+  <si>
+    <t>Wayne County: County Forecast</t>
+  </si>
+  <si>
+    <t>Wayne County: Live Doppler</t>
+  </si>
+  <si>
+    <t>WHIO</t>
   </si>
 </sst>
 </file>
@@ -716,17 +1031,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D54A8C-5D99-5240-A81E-2135DEC62769}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="N74" sqref="N74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1256,6 +1571,592 @@
       <c r="C48" s="1" t="s">
         <v>76</v>
       </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>203</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>203</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>203</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>203</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>203</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>203</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>203</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>203</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>203</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>203</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>203</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>203</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>203</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>203</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>203</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>203</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>203</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>203</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>203</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>203</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>203</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>203</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>203</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>203</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>203</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>203</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>203</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>203</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>203</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>203</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>203</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>203</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>203</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>203</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>203</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>203</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>203</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>203</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>203</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>203</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>203</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>203</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>203</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>203</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>203</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>203</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>203</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>203</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>203</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>203</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>203</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B102" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1306,6 +2207,59 @@
     <hyperlink ref="C46" r:id="rId45" xr:uid="{C82A0A61-33D1-3745-BAD7-077A9534B631}"/>
     <hyperlink ref="C47" r:id="rId46" xr:uid="{A82D619F-F86A-1244-AC1A-DF304756670C}"/>
     <hyperlink ref="C48" r:id="rId47" xr:uid="{6844DE22-6E0A-654C-8351-45ADA5D96C8B}"/>
+    <hyperlink ref="C49" r:id="rId48" xr:uid="{DD45B488-F311-0B4B-877B-70CB66E82451}"/>
+    <hyperlink ref="C50" r:id="rId49" display="https://mediaweb.whio.com/weather/Auglaize Co Temps.jpg" xr:uid="{BC717921-5FCE-1145-84E7-B094937DC27D}"/>
+    <hyperlink ref="C51" r:id="rId50" display="https://mediaweb.whio.com/weather/Auglaize Co Today.jpg" xr:uid="{9DEC9C25-7275-3C4A-8A14-9E52233C734C}"/>
+    <hyperlink ref="C52" r:id="rId51" display="https://mediaweb.whio.com/weather/Auglaize County Radar.jpg" xr:uid="{B6E0911C-2891-F34F-B6EC-D0BFF7A9C39F}"/>
+    <hyperlink ref="C53" r:id="rId52" display="https://mediaweb.whio.com/weather/Butler Co Temps .jpg" xr:uid="{62FB33CA-373C-DE41-8D1A-030581D36149}"/>
+    <hyperlink ref="C54" r:id="rId53" display="https://mediaweb.whio.com/weather/Butler Co Today.jpg" xr:uid="{B74EB7D4-B24F-6748-BD10-0CCD58DBC3E4}"/>
+    <hyperlink ref="C55" r:id="rId54" display="https://mediaweb.whio.com/weather/Butler County Radar.jpg" xr:uid="{3356CF4D-6C90-DB4B-86A7-43295EF5FF98}"/>
+    <hyperlink ref="C56" r:id="rId55" display="https://mediaweb.whio.com/weather/Champaign Co Temperatures.jpg" xr:uid="{12B6FB3C-3AC0-2946-ADFC-26C6FC4BE3B2}"/>
+    <hyperlink ref="C57" r:id="rId56" display="https://mediaweb.whio.com/weather/Champaign Co Today.jpg" xr:uid="{EC6723F0-C914-5E4A-8CE4-60E1B0CAEFB3}"/>
+    <hyperlink ref="C58" r:id="rId57" display="https://mediaweb.whio.com/weather/Champain County Radar.jpg" xr:uid="{62AEAFEA-8188-CA4E-9483-DA6591FB238F}"/>
+    <hyperlink ref="C59" r:id="rId58" display="https://mediaweb.whio.com/weather/Clark Co Temps.jpg" xr:uid="{77E3480B-FD2C-B249-A0F8-EEB9F6C385B1}"/>
+    <hyperlink ref="C60" r:id="rId59" display="https://mediaweb.whio.com/weather/Clark Co Today .png" xr:uid="{825D13E2-E9EF-FF47-8221-DB318EA6AB3B}"/>
+    <hyperlink ref="C61" r:id="rId60" display="https://mediaweb.whio.com/weather/Clark County Radar.jpg" xr:uid="{CDB640D1-67C3-B442-AD39-3F0743A4CA41}"/>
+    <hyperlink ref="C62" r:id="rId61" display="https://mediaweb.whio.com/weather/Darke Co Temps.jpg" xr:uid="{760517AD-3EC8-7849-8C13-FBC694EC11C1}"/>
+    <hyperlink ref="C63" r:id="rId62" display="https://mediaweb.whio.com/weather/Darke Co Today .jpg" xr:uid="{4E646B63-A09F-EC4E-96E5-F179FB4FBF7D}"/>
+    <hyperlink ref="C64" r:id="rId63" display="https://mediaweb.whio.com/weather/Darke County Radar.jpg" xr:uid="{2E7E3AB4-C2A6-0B4D-A72C-FDAB80BFF1F9}"/>
+    <hyperlink ref="C65" r:id="rId64" display="https://mediaweb.whio.com/weather/DMA Visibility.jpg" xr:uid="{641D3953-DB34-474B-869B-113990748CFF}"/>
+    <hyperlink ref="C66" r:id="rId65" display="https://mediaweb.whio.com/weather/DMA Watches Warnings.jpg" xr:uid="{22487487-7821-7C46-98C0-8F6E4122B01A}"/>
+    <hyperlink ref="C67" r:id="rId66" display="https://mediaweb.whio.com/weather/Greene Co Temps .jpg" xr:uid="{2F282EF8-8B35-B946-A874-E8D367EBCA15}"/>
+    <hyperlink ref="C68" r:id="rId67" display="https://mediaweb.whio.com/weather/Greene Co Today.jpg" xr:uid="{A2BF9CED-31F6-1244-86E3-0B9BE9B01203}"/>
+    <hyperlink ref="C69" r:id="rId68" display="https://mediaweb.whio.com/weather/Greene County Radar.jpg" xr:uid="{5F7A2E8D-7D48-A34E-A4B9-50088E5C4756}"/>
+    <hyperlink ref="C70" r:id="rId69" display="https://mediaweb.whio.com/weather/Live Doppler 7.jpg" xr:uid="{9E6C0B63-2C46-804A-A4AA-488B902096F2}"/>
+    <hyperlink ref="C71" r:id="rId70" display="https://mediaweb.whio.com/weather/Logan Co Temps .jpg" xr:uid="{7652FFA8-8CDC-CC4A-9CDB-0CD25ABFB866}"/>
+    <hyperlink ref="C72" r:id="rId71" display="https://mediaweb.whio.com/weather/Logan Co Today.jpg" xr:uid="{8C79DFC8-18A0-BB4C-9096-7606532BC715}"/>
+    <hyperlink ref="C73" r:id="rId72" display="https://mediaweb.whio.com/weather/Logan County Radar.png" xr:uid="{0A3F6713-2C09-D048-AE94-313A9A0F3174}"/>
+    <hyperlink ref="C74" r:id="rId73" display="https://mediaweb.whio.com/weather/Mercer Co Temps .jpg" xr:uid="{8AFFD2BE-E7A6-0F4B-A0C1-1FF84514B4DC}"/>
+    <hyperlink ref="C75" r:id="rId74" display="https://mediaweb.whio.com/weather/Mercer Co Today .jpg" xr:uid="{CD975B53-E116-C34B-816D-ED87D9F37F25}"/>
+    <hyperlink ref="C76" r:id="rId75" display="https://mediaweb.whio.com/weather/Mercer County Radar.jpg" xr:uid="{19E92440-F293-8642-B706-A2346C42AC5B}"/>
+    <hyperlink ref="C77" r:id="rId76" display="https://mediaweb.whio.com/weather/Miami Co Temps.jpg" xr:uid="{003BA2D1-5327-BA41-BB1A-3DD17C26E520}"/>
+    <hyperlink ref="C78" r:id="rId77" display="https://mediaweb.whio.com/weather/Miami Co Today.jpg" xr:uid="{3F2EDC65-B7A0-DA48-910C-D11FF68F67BC}"/>
+    <hyperlink ref="C79" r:id="rId78" display="https://mediaweb.whio.com/weather/Miami County Radar.jpg" xr:uid="{DFF7B593-7EED-4844-8051-25F4FC0D349A}"/>
+    <hyperlink ref="C80" r:id="rId79" display="https://mediaweb.whio.com/weather/Miami Valley Temps.jpg" xr:uid="{282B13EF-4C09-EE4A-8E78-1CC510EBBE88}"/>
+    <hyperlink ref="C81" r:id="rId80" display="https://mediaweb.whio.com/weather/Miami Valley Wind Speed.jpg" xr:uid="{C9469A71-0C26-8344-B8B5-7A302B62A510}"/>
+    <hyperlink ref="C82" r:id="rId81" display="https://mediaweb.whio.com/weather/Montgomery Co Temps .jpg" xr:uid="{FDD0BEC1-0490-F142-B2F6-F2EA9C9E4F78}"/>
+    <hyperlink ref="C83" r:id="rId82" display="https://mediaweb.whio.com/weather/Montgomery Co Today.jpg" xr:uid="{6E0BB2A5-C22C-4D4C-AEDE-E3A55FDAFA6A}"/>
+    <hyperlink ref="C84" r:id="rId83" display="https://mediaweb.whio.com/weather/Montgomery County Radar.jpg" xr:uid="{AC871DDC-57A5-534A-AC81-04EFE51F5404}"/>
+    <hyperlink ref="C85" r:id="rId84" display="https://mediaweb.whio.com/weather/National Airport Delays.jpg" xr:uid="{C708EF1B-04F8-494C-9E0E-E64AA268CCFB}"/>
+    <hyperlink ref="C86" r:id="rId85" display="https://mediaweb.whio.com/weather/National SatRad.jpg" xr:uid="{1D647BBB-0EE4-8A44-B47B-232F585A6C5C}"/>
+    <hyperlink ref="C87" r:id="rId86" display="https://mediaweb.whio.com/weather/Preble Co Temps.jpg" xr:uid="{278FF1EE-8776-AF46-919E-5318B5061DB5}"/>
+    <hyperlink ref="C88" r:id="rId87" display="https://mediaweb.whio.com/weather/Preble Co Today.jpg" xr:uid="{16E8C2EA-0A0D-AB41-8581-23A3C4B2C23B}"/>
+    <hyperlink ref="C89" r:id="rId88" display="https://mediaweb.whio.com/weather/Preble County Radar.jpg" xr:uid="{BB36C583-0F81-014B-8ECB-CC17902AD223}"/>
+    <hyperlink ref="C90" r:id="rId89" display="https://mediaweb.whio.com/weather/Redional SatRad .jpg" xr:uid="{0794FC70-A2A1-3944-B22E-E608EBBD9022}"/>
+    <hyperlink ref="C91" r:id="rId90" display="https://mediaweb.whio.com/weather/Redional SatRad .jpg" xr:uid="{B0719C96-0C82-A341-A547-E52AF57E35F5}"/>
+    <hyperlink ref="C92" r:id="rId91" display="https://mediaweb.whio.com/weather/Regional Airport Delays.jpg" xr:uid="{FA042336-A2E6-DF4D-BE08-575835B4FD95}"/>
+    <hyperlink ref="C93" r:id="rId92" display="https://mediaweb.whio.com/weather/Shelby Co Temps .jpg" xr:uid="{D7367F68-27E5-0041-B4EC-C941785915D3}"/>
+    <hyperlink ref="C94" r:id="rId93" display="https://mediaweb.whio.com/weather/Shelby Co Today .jpg" xr:uid="{B0D19F99-269B-BF44-BCC7-D8E1343EAFDA}"/>
+    <hyperlink ref="C95" r:id="rId94" display="https://mediaweb.whio.com/weather/Shelby County Radar.jpg" xr:uid="{EAAC411D-6604-874A-848C-F1D10F80D763}"/>
+    <hyperlink ref="C96" r:id="rId95" display="https://mediaweb.whio.com/weather/Warren Co Temps .jpg" xr:uid="{73454399-6FC2-084F-9A31-7EAE0F22925C}"/>
+    <hyperlink ref="C97" r:id="rId96" display="https://mediaweb.whio.com/weather/Warren Co Today.jpg" xr:uid="{0BEA5401-AB97-7F4A-9470-FC60E42D8218}"/>
+    <hyperlink ref="C98" r:id="rId97" display="https://mediaweb.whio.com/weather/Warren County Radar.jpg" xr:uid="{EE38F76F-3F84-B240-ABE4-83CCA3425364}"/>
+    <hyperlink ref="C99" r:id="rId98" display="https://mediaweb.whio.com/weather/Wayne Co Temps.jpg" xr:uid="{B94018DA-652E-FB49-8BA2-FAF4A948703C}"/>
+    <hyperlink ref="C100" r:id="rId99" display="https://mediaweb.whio.com/weather/Wayne Co Today .jpg" xr:uid="{BD533EED-4BE6-9F49-957D-CEE45FD433D3}"/>
+    <hyperlink ref="C101" r:id="rId100" display="https://mediaweb.whio.com/weather/Wayne County Radar.jpg" xr:uid="{13A42CFE-5B51-554E-8252-90CC8A127EE9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[master] Added a new wxGroup parameter for the slideshow images to group them by
</commit_message>
<xml_diff>
--- a/src/Components/data/wx-images.xlsx
+++ b/src/Components/data/wx-images.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maysamheydari/amagi-poc/src/Components/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D104D138-B40B-2848-96EF-CC971166BA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5410BBFC-9453-3A48-9E6E-0582D7A30093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="11840" windowWidth="38400" windowHeight="21600" xr2:uid="{27725300-7AC2-F649-856A-4042AE1EE323}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="206">
   <si>
     <t>site</t>
   </si>
@@ -647,6 +647,12 @@
   </si>
   <si>
     <t>WHIO</t>
+  </si>
+  <si>
+    <t>wxGroup</t>
+  </si>
+  <si>
+    <t>days</t>
   </si>
 </sst>
 </file>
@@ -1031,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D54A8C-5D99-5240-A81E-2135DEC62769}">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="N74" sqref="N74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1044,7 +1050,7 @@
     <col min="3" max="3" width="68.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1054,8 +1060,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1065,8 +1074,11 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1076,8 +1088,11 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1087,8 +1102,11 @@
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1098,8 +1116,11 @@
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1109,8 +1130,11 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1120,8 +1144,11 @@
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1131,8 +1158,11 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1142,8 +1172,11 @@
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1153,8 +1186,11 @@
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1164,8 +1200,11 @@
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1175,8 +1214,11 @@
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1186,8 +1228,11 @@
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1197,8 +1242,11 @@
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1208,8 +1256,11 @@
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1219,8 +1270,11 @@
       <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1230,8 +1284,11 @@
       <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -1241,8 +1298,11 @@
       <c r="C18" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1252,8 +1312,11 @@
       <c r="C19" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -1263,8 +1326,11 @@
       <c r="C20" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1274,8 +1340,11 @@
       <c r="C21" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -1285,8 +1354,11 @@
       <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -1296,8 +1368,11 @@
       <c r="C23" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -1307,8 +1382,11 @@
       <c r="C24" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -1318,8 +1396,11 @@
       <c r="C25" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -1329,8 +1410,11 @@
       <c r="C26" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -1340,8 +1424,11 @@
       <c r="C27" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>98</v>
       </c>
@@ -1351,8 +1438,11 @@
       <c r="C28" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>98</v>
       </c>
@@ -1362,8 +1452,11 @@
       <c r="C29" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>98</v>
       </c>
@@ -1373,8 +1466,11 @@
       <c r="C30" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -1384,8 +1480,11 @@
       <c r="C31" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -1395,8 +1494,11 @@
       <c r="C32" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -1406,8 +1508,11 @@
       <c r="C33" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>98</v>
       </c>
@@ -1417,8 +1522,11 @@
       <c r="C34" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>98</v>
       </c>
@@ -1428,8 +1536,11 @@
       <c r="C35" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>98</v>
       </c>
@@ -1439,8 +1550,11 @@
       <c r="C36" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -1450,8 +1564,11 @@
       <c r="C37" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -1461,8 +1578,11 @@
       <c r="C38" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -1472,8 +1592,11 @@
       <c r="C39" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>98</v>
       </c>
@@ -1483,8 +1606,11 @@
       <c r="C40" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -1494,8 +1620,11 @@
       <c r="C41" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -1505,8 +1634,11 @@
       <c r="C42" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -1516,8 +1648,11 @@
       <c r="C43" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -1527,8 +1662,11 @@
       <c r="C44" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -1538,8 +1676,11 @@
       <c r="C45" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>98</v>
       </c>
@@ -1549,8 +1690,11 @@
       <c r="C46" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -1560,8 +1704,11 @@
       <c r="C47" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -1571,8 +1718,11 @@
       <c r="C48" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>203</v>
       </c>
@@ -1582,8 +1732,11 @@
       <c r="C49" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>203</v>
       </c>
@@ -1593,8 +1746,11 @@
       <c r="C50" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>203</v>
       </c>
@@ -1604,8 +1760,11 @@
       <c r="C51" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>203</v>
       </c>
@@ -1615,8 +1774,11 @@
       <c r="C52" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>203</v>
       </c>
@@ -1626,8 +1788,11 @@
       <c r="C53" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>203</v>
       </c>
@@ -1637,8 +1802,11 @@
       <c r="C54" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>203</v>
       </c>
@@ -1648,8 +1816,11 @@
       <c r="C55" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>203</v>
       </c>
@@ -1659,8 +1830,11 @@
       <c r="C56" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>203</v>
       </c>
@@ -1670,8 +1844,11 @@
       <c r="C57" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>203</v>
       </c>
@@ -1681,8 +1858,11 @@
       <c r="C58" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>203</v>
       </c>
@@ -1692,8 +1872,11 @@
       <c r="C59" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>203</v>
       </c>
@@ -1703,8 +1886,11 @@
       <c r="C60" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>203</v>
       </c>
@@ -1714,8 +1900,11 @@
       <c r="C61" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>203</v>
       </c>
@@ -1725,8 +1914,11 @@
       <c r="C62" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>203</v>
       </c>
@@ -1736,8 +1928,11 @@
       <c r="C63" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>203</v>
       </c>
@@ -1747,8 +1942,11 @@
       <c r="C64" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>203</v>
       </c>
@@ -1758,8 +1956,11 @@
       <c r="C65" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>203</v>
       </c>
@@ -1769,8 +1970,11 @@
       <c r="C66" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>203</v>
       </c>
@@ -1780,8 +1984,11 @@
       <c r="C67" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>203</v>
       </c>
@@ -1791,8 +1998,11 @@
       <c r="C68" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>203</v>
       </c>
@@ -1802,8 +2012,11 @@
       <c r="C69" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>203</v>
       </c>
@@ -1813,8 +2026,11 @@
       <c r="C70" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>203</v>
       </c>
@@ -1824,8 +2040,11 @@
       <c r="C71" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>203</v>
       </c>
@@ -1835,8 +2054,11 @@
       <c r="C72" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>203</v>
       </c>
@@ -1846,8 +2068,11 @@
       <c r="C73" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>203</v>
       </c>
@@ -1857,8 +2082,11 @@
       <c r="C74" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>203</v>
       </c>
@@ -1868,8 +2096,11 @@
       <c r="C75" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>203</v>
       </c>
@@ -1879,8 +2110,11 @@
       <c r="C76" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>203</v>
       </c>
@@ -1890,8 +2124,11 @@
       <c r="C77" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>203</v>
       </c>
@@ -1901,8 +2138,11 @@
       <c r="C78" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>203</v>
       </c>
@@ -1912,8 +2152,11 @@
       <c r="C79" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>203</v>
       </c>
@@ -1923,8 +2166,11 @@
       <c r="C80" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>203</v>
       </c>
@@ -1934,8 +2180,11 @@
       <c r="C81" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>203</v>
       </c>
@@ -1945,8 +2194,11 @@
       <c r="C82" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>203</v>
       </c>
@@ -1956,8 +2208,11 @@
       <c r="C83" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>203</v>
       </c>
@@ -1967,8 +2222,11 @@
       <c r="C84" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>203</v>
       </c>
@@ -1978,8 +2236,11 @@
       <c r="C85" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>203</v>
       </c>
@@ -1989,8 +2250,11 @@
       <c r="C86" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>203</v>
       </c>
@@ -2000,8 +2264,11 @@
       <c r="C87" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>203</v>
       </c>
@@ -2011,8 +2278,11 @@
       <c r="C88" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>203</v>
       </c>
@@ -2022,8 +2292,11 @@
       <c r="C89" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>203</v>
       </c>
@@ -2033,8 +2306,11 @@
       <c r="C90" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>203</v>
       </c>
@@ -2044,8 +2320,11 @@
       <c r="C91" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>203</v>
       </c>
@@ -2055,8 +2334,11 @@
       <c r="C92" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>203</v>
       </c>
@@ -2066,8 +2348,11 @@
       <c r="C93" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>203</v>
       </c>
@@ -2077,8 +2362,11 @@
       <c r="C94" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>203</v>
       </c>
@@ -2088,8 +2376,11 @@
       <c r="C95" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>203</v>
       </c>
@@ -2099,8 +2390,11 @@
       <c r="C96" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>203</v>
       </c>
@@ -2110,8 +2404,11 @@
       <c r="C97" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>203</v>
       </c>
@@ -2121,8 +2418,11 @@
       <c r="C98" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>203</v>
       </c>
@@ -2132,8 +2432,11 @@
       <c r="C99" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>203</v>
       </c>
@@ -2143,8 +2446,11 @@
       <c r="C100" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>203</v>
       </c>
@@ -2154,8 +2460,11 @@
       <c r="C101" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B102" s="2"/>
     </row>
   </sheetData>

</xml_diff>